<commit_message>
New Changes on network
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1056,7 +1056,7 @@
     <row r="16" ht="15" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
-          <t>software Peyton</t>
+          <t>software Riley</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>MarketingPeyton</t>
+          <t>MarketingRiley</t>
         </is>
       </c>
     </row>

</xml_diff>